<commit_message>
add decimal field to
</commit_message>
<xml_diff>
--- a/bot/handlers/reports/xlsx/panasonic_default_sales_data.xlsx
+++ b/bot/handlers/reports/xlsx/panasonic_default_sales_data.xlsx
@@ -1236,7 +1236,7 @@
     <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1248,9 +1248,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -1730,16 +1735,13 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1748,125 +1750,131 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2211,7 +2219,7 @@
   <dimension ref="A1:D287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -2236,7 +2244,7 @@
       <c r="A2" s="3">
         <v>91400001</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3">
@@ -2247,7 +2255,7 @@
       <c r="A3" s="3">
         <v>91400002</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3">
@@ -2258,7 +2266,7 @@
       <c r="A4" s="3">
         <v>90400003</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3">
@@ -2269,7 +2277,7 @@
       <c r="A5" s="3">
         <v>91400068</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3">
@@ -2280,7 +2288,7 @@
       <c r="A6" s="3">
         <v>91400004</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="3">
@@ -2291,7 +2299,7 @@
       <c r="A7" s="3">
         <v>91400017</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3">
@@ -2302,7 +2310,7 @@
       <c r="A8" s="3">
         <v>91400006</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3">
@@ -2313,7 +2321,7 @@
       <c r="A9" s="3">
         <v>91400031</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3">
@@ -2324,7 +2332,7 @@
       <c r="A10" s="3">
         <v>91400020</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="3">
@@ -2335,7 +2343,7 @@
       <c r="A11" s="3">
         <v>91400007</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="3">
@@ -2346,7 +2354,7 @@
       <c r="A12" s="3">
         <v>91400008</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="3">
@@ -2357,7 +2365,7 @@
       <c r="A13" s="3">
         <v>91400055</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3">
@@ -2368,7 +2376,7 @@
       <c r="A14" s="3">
         <v>91400056</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="3">
@@ -2379,7 +2387,7 @@
       <c r="A15" s="3">
         <v>91400012</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="3">
@@ -2390,7 +2398,7 @@
       <c r="A16" s="3">
         <v>91400010</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="3">
@@ -2401,7 +2409,7 @@
       <c r="A17" s="3">
         <v>91400013</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="3">
@@ -2412,7 +2420,7 @@
       <c r="A18" s="3">
         <v>91400032</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="3">
@@ -2423,7 +2431,7 @@
       <c r="A19" s="3">
         <v>91400034</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3">
@@ -2434,7 +2442,7 @@
       <c r="A20" s="3">
         <v>91400035</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="3">
@@ -2445,7 +2453,7 @@
       <c r="A21" s="3">
         <v>91480002</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="3">
@@ -2456,7 +2464,7 @@
       <c r="A22" s="3">
         <v>91480003</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="3">
@@ -2467,7 +2475,7 @@
       <c r="A23" s="3">
         <v>91480004</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="3">
@@ -2478,7 +2486,7 @@
       <c r="A24" s="3">
         <v>91480005</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="3">
@@ -2489,7 +2497,7 @@
       <c r="A25" s="3">
         <v>91480006</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="3">
@@ -2500,7 +2508,7 @@
       <c r="A26" s="3">
         <v>91480008</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="3">
@@ -2518,7 +2526,7 @@
       <c r="A28" s="3">
         <v>90561001</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="3">
@@ -2529,7 +2537,7 @@
       <c r="A29" s="3">
         <v>90561002</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="3">
@@ -2540,7 +2548,7 @@
       <c r="A30" s="3">
         <v>90561068</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="3">
@@ -2551,7 +2559,7 @@
       <c r="A31" s="3">
         <v>90561004</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="3">
@@ -2562,7 +2570,7 @@
       <c r="A32" s="3">
         <v>90561017</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="3">
@@ -2573,7 +2581,7 @@
       <c r="A33" s="3">
         <v>90561083</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="3">
@@ -2584,7 +2592,7 @@
       <c r="A34" s="3">
         <v>90561031</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="3">
@@ -2595,7 +2603,7 @@
       <c r="A35" s="3">
         <v>90561006</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="3">
@@ -2606,7 +2614,7 @@
       <c r="A36" s="3">
         <v>90561020</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="3">
@@ -2617,7 +2625,7 @@
       <c r="A37" s="3">
         <v>90561069</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="3">
@@ -2628,7 +2636,7 @@
       <c r="A38" s="3">
         <v>90561007</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="3">
@@ -2639,7 +2647,7 @@
       <c r="A39" s="3">
         <v>90561008</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="3">
@@ -2650,7 +2658,7 @@
       <c r="A40" s="3">
         <v>90561043</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="3">
@@ -2661,7 +2669,7 @@
       <c r="A41" s="3">
         <v>90561042</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="3">
@@ -2672,7 +2680,7 @@
       <c r="A42" s="3">
         <v>90561055</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="3">
@@ -2683,7 +2691,7 @@
       <c r="A43" s="3">
         <v>90561056</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="3">
@@ -2694,7 +2702,7 @@
       <c r="A44" s="3">
         <v>90561012</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C44" s="3">
@@ -2705,7 +2713,7 @@
       <c r="A45" s="3">
         <v>90561049</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C45" s="3">
@@ -2716,7 +2724,7 @@
       <c r="A46" s="3">
         <v>90561010</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="3">
@@ -2727,7 +2735,7 @@
       <c r="A47" s="3">
         <v>90561013</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C47" s="3">
@@ -2738,7 +2746,7 @@
       <c r="A48" s="3">
         <v>90561033</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C48" s="3">
@@ -2749,7 +2757,7 @@
       <c r="A49" s="3">
         <v>90561011</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C49" s="3">
@@ -2760,7 +2768,7 @@
       <c r="A50" s="3">
         <v>90561032</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C50" s="3">
@@ -2771,7 +2779,7 @@
       <c r="A51" s="3">
         <v>90561034</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="3">
@@ -2782,7 +2790,7 @@
       <c r="A52" s="3">
         <v>90561035</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C52" s="3">
@@ -2793,7 +2801,7 @@
       <c r="A53" s="3">
         <v>90571102</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C53" s="3">
@@ -2804,7 +2812,7 @@
       <c r="A54" s="3">
         <v>90571103</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C54" s="3">
@@ -2815,7 +2823,7 @@
       <c r="A55" s="3">
         <v>90571104</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C55" s="3">
@@ -2826,7 +2834,7 @@
       <c r="A56" s="3">
         <v>90571105</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C56" s="3">
@@ -2837,7 +2845,7 @@
       <c r="A57" s="3">
         <v>90571106</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C57" s="3">
@@ -2848,7 +2856,7 @@
       <c r="A58" s="3">
         <v>90571002</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C58" s="3">
@@ -2859,7 +2867,7 @@
       <c r="A59" s="3">
         <v>90571003</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C59" s="3">
@@ -2870,7 +2878,7 @@
       <c r="A60" s="3">
         <v>90571009</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C60" s="3">
@@ -2888,7 +2896,7 @@
       <c r="A62" s="3">
         <v>90960001</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C62" s="3">
@@ -2899,7 +2907,7 @@
       <c r="A63" s="3">
         <v>90960002</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C63" s="3">
@@ -2910,7 +2918,7 @@
       <c r="A64" s="3">
         <v>90960068</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C64" s="3">
@@ -2921,7 +2929,7 @@
       <c r="A65" s="3">
         <v>90960004</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C65" s="3">
@@ -2932,7 +2940,7 @@
       <c r="A66" s="3">
         <v>90960017</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C66" s="3">
@@ -2943,7 +2951,7 @@
       <c r="A67" s="3">
         <v>90960083</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C67" s="3">
@@ -2954,7 +2962,7 @@
       <c r="A68" s="3">
         <v>90960031</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C68" s="3">
@@ -2965,7 +2973,7 @@
       <c r="A69" s="3">
         <v>90960020</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C69" s="3">
@@ -2976,7 +2984,7 @@
       <c r="A70" s="3">
         <v>90960069</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C70" s="3">
@@ -2987,7 +2995,7 @@
       <c r="A71" s="3">
         <v>90960003</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C71" s="3">
@@ -2998,7 +3006,7 @@
       <c r="A72" s="3">
         <v>90960006</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C72" s="3">
@@ -3009,7 +3017,7 @@
       <c r="A73" s="3">
         <v>90960007</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C73" s="3">
@@ -3020,7 +3028,7 @@
       <c r="A74" s="3">
         <v>90960008</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C74" s="3">
@@ -3031,7 +3039,7 @@
       <c r="A75" s="3">
         <v>90960055</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C75" s="3">
@@ -3042,7 +3050,7 @@
       <c r="A76" s="3">
         <v>90960056</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C76" s="3">
@@ -3053,7 +3061,7 @@
       <c r="A77" s="3">
         <v>90960012</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C77" s="3">
@@ -3064,7 +3072,7 @@
       <c r="A78" s="3">
         <v>90960010</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C78" s="3">
@@ -3075,7 +3083,7 @@
       <c r="A79" s="3">
         <v>90960013</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C79" s="3">
@@ -3086,7 +3094,7 @@
       <c r="A80" s="3">
         <v>90960033</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C80" s="3">
@@ -3097,7 +3105,7 @@
       <c r="A81" s="3">
         <v>90961017</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="4" t="s">
         <v>82</v>
       </c>
       <c r="C81" s="3">
@@ -3108,7 +3116,7 @@
       <c r="A82" s="3">
         <v>90960032</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C82" s="3">
@@ -3119,7 +3127,7 @@
       <c r="A83" s="3">
         <v>90960034</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C83" s="3">
@@ -3130,7 +3138,7 @@
       <c r="A84" s="3">
         <v>90960035</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C84" s="3">
@@ -3141,7 +3149,7 @@
       <c r="A85" s="3">
         <v>90961008</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C85" s="3">
@@ -3152,7 +3160,7 @@
       <c r="A86" s="3">
         <v>90960201</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C86" s="3">
@@ -3163,7 +3171,7 @@
       <c r="A87" s="3">
         <v>90960202</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="4" t="s">
         <v>88</v>
       </c>
       <c r="C87" s="3">
@@ -3174,7 +3182,7 @@
       <c r="A88" s="3">
         <v>90960203</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C88" s="3">
@@ -3185,7 +3193,7 @@
       <c r="A89" s="3">
         <v>90960204</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="4" t="s">
         <v>90</v>
       </c>
       <c r="C89" s="3">
@@ -3196,7 +3204,7 @@
       <c r="A90" s="3">
         <v>90960205</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C90" s="3">
@@ -3207,7 +3215,7 @@
       <c r="A91" s="3">
         <v>90969003</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C91" s="3">
@@ -3218,7 +3226,7 @@
       <c r="A92" s="3">
         <v>90961004</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="4" t="s">
         <v>93</v>
       </c>
       <c r="C92" s="3">
@@ -3233,10 +3241,10 @@
       <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="4" t="s">
         <v>96</v>
       </c>
       <c r="C94" s="3">
@@ -3244,10 +3252,10 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C95" s="3">
@@ -3255,10 +3263,10 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C96" s="3">
@@ -3266,10 +3274,10 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="4" t="s">
         <v>102</v>
       </c>
       <c r="C97" s="3">
@@ -3277,10 +3285,10 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="4" t="s">
         <v>104</v>
       </c>
       <c r="C98" s="3">
@@ -3288,10 +3296,10 @@
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C99" s="3">
@@ -3299,10 +3307,10 @@
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C100" s="3">
@@ -3310,10 +3318,10 @@
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C101" s="3">
@@ -3321,10 +3329,10 @@
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="4" t="s">
         <v>112</v>
       </c>
       <c r="C102" s="3">
@@ -3332,10 +3340,10 @@
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C103" s="3">
@@ -3343,10 +3351,10 @@
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C104" s="3">
@@ -3354,10 +3362,10 @@
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C105" s="3">
@@ -3365,10 +3373,10 @@
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="4" t="s">
         <v>120</v>
       </c>
       <c r="C106" s="3">
@@ -3376,10 +3384,10 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B107" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C107" s="3">
@@ -3387,10 +3395,10 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="4" t="s">
         <v>124</v>
       </c>
       <c r="C108" s="3">
@@ -3398,10 +3406,10 @@
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="4" t="s">
         <v>126</v>
       </c>
       <c r="C109" s="3">
@@ -3409,10 +3417,10 @@
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="4" t="s">
         <v>128</v>
       </c>
       <c r="C110" s="3">
@@ -3420,10 +3428,10 @@
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="4" t="s">
         <v>130</v>
       </c>
       <c r="C111" s="3">
@@ -3431,10 +3439,10 @@
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="4" t="s">
         <v>132</v>
       </c>
       <c r="C112" s="3">
@@ -3442,10 +3450,10 @@
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="4" t="s">
         <v>134</v>
       </c>
       <c r="C113" s="3">
@@ -3453,10 +3461,10 @@
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C114" s="3">
@@ -3464,10 +3472,10 @@
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="4" t="s">
         <v>138</v>
       </c>
       <c r="C115" s="3">
@@ -3475,10 +3483,10 @@
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="3" t="s">
+      <c r="A116" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="4" t="s">
         <v>140</v>
       </c>
       <c r="C116" s="3">
@@ -3486,10 +3494,10 @@
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C117" s="3">
@@ -3497,10 +3505,10 @@
       </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="4" t="s">
         <v>144</v>
       </c>
       <c r="C118" s="3">
@@ -3508,10 +3516,10 @@
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="4" t="s">
         <v>146</v>
       </c>
       <c r="C119" s="3">
@@ -3519,10 +3527,10 @@
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="4" t="s">
         <v>148</v>
       </c>
       <c r="C120" s="3">
@@ -3530,10 +3538,10 @@
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="3" t="s">
+      <c r="A121" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="4" t="s">
         <v>150</v>
       </c>
       <c r="C121" s="3">
@@ -3548,10 +3556,10 @@
       <c r="C122" s="1"/>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="4" t="s">
         <v>153</v>
       </c>
       <c r="C123" s="3">
@@ -3559,10 +3567,10 @@
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="4" t="s">
         <v>155</v>
       </c>
       <c r="C124" s="3">
@@ -3570,10 +3578,10 @@
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="3" t="s">
+      <c r="A125" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="4" t="s">
         <v>157</v>
       </c>
       <c r="C125" s="3">
@@ -3581,10 +3589,10 @@
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="3" t="s">
+      <c r="A126" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B126" s="4" t="s">
         <v>159</v>
       </c>
       <c r="C126" s="3">
@@ -3592,10 +3600,10 @@
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B127" s="4" t="s">
         <v>161</v>
       </c>
       <c r="C127" s="3">
@@ -3603,10 +3611,10 @@
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" s="4" t="s">
         <v>163</v>
       </c>
       <c r="C128" s="3">
@@ -3614,10 +3622,10 @@
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="3" t="s">
+      <c r="A129" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B129" s="4" t="s">
         <v>165</v>
       </c>
       <c r="C129" s="3">
@@ -3625,10 +3633,10 @@
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="3" t="s">
+      <c r="A130" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B130" s="4" t="s">
         <v>167</v>
       </c>
       <c r="C130" s="3">
@@ -3636,10 +3644,10 @@
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="B131" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C131" s="3">
@@ -3647,10 +3655,10 @@
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="3" t="s">
+      <c r="A132" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B132" s="4" t="s">
         <v>171</v>
       </c>
       <c r="C132" s="3">
@@ -3658,10 +3666,10 @@
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="3" t="s">
+      <c r="A133" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B133" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C133" s="3">
@@ -3669,10 +3677,10 @@
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="3" t="s">
+      <c r="A134" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B134" s="3" t="s">
+      <c r="B134" s="4" t="s">
         <v>175</v>
       </c>
       <c r="C134" s="3">
@@ -3680,10 +3688,10 @@
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="B135" s="4" t="s">
         <v>177</v>
       </c>
       <c r="C135" s="3">
@@ -3691,10 +3699,10 @@
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="3" t="s">
+      <c r="A136" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B136" s="4" t="s">
         <v>179</v>
       </c>
       <c r="C136" s="3">
@@ -3702,10 +3710,10 @@
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B137" s="4" t="s">
         <v>181</v>
       </c>
       <c r="C137" s="3">
@@ -3713,10 +3721,10 @@
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="3" t="s">
+      <c r="A138" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B138" s="3" t="s">
+      <c r="B138" s="4" t="s">
         <v>183</v>
       </c>
       <c r="C138" s="3">
@@ -3724,10 +3732,10 @@
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="3" t="s">
+      <c r="A139" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="B139" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C139" s="3">
@@ -3735,10 +3743,10 @@
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="3" t="s">
+      <c r="A140" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B140" s="3" t="s">
+      <c r="B140" s="4" t="s">
         <v>187</v>
       </c>
       <c r="C140" s="3">
@@ -3746,10 +3754,10 @@
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="3" t="s">
+      <c r="A141" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B141" s="3" t="s">
+      <c r="B141" s="4" t="s">
         <v>189</v>
       </c>
       <c r="C141" s="3">
@@ -3757,10 +3765,10 @@
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="3" t="s">
+      <c r="A142" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B142" s="3" t="s">
+      <c r="B142" s="4" t="s">
         <v>191</v>
       </c>
       <c r="C142" s="3">
@@ -3768,10 +3776,10 @@
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="3" t="s">
+      <c r="A143" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B143" s="3" t="s">
+      <c r="B143" s="4" t="s">
         <v>193</v>
       </c>
       <c r="C143" s="3">
@@ -3779,10 +3787,10 @@
       </c>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B144" s="4" t="s">
         <v>195</v>
       </c>
       <c r="C144" s="3">
@@ -3790,10 +3798,10 @@
       </c>
     </row>
     <row r="145" spans="1:3">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="B145" s="4" t="s">
         <v>197</v>
       </c>
       <c r="C145" s="3">
@@ -3801,10 +3809,10 @@
       </c>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B146" s="3" t="s">
+      <c r="B146" s="4" t="s">
         <v>199</v>
       </c>
       <c r="C146" s="3">
@@ -3812,10 +3820,10 @@
       </c>
     </row>
     <row r="147" spans="1:3">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B147" s="4" t="s">
         <v>201</v>
       </c>
       <c r="C147" s="3">
@@ -3826,7 +3834,7 @@
       <c r="A148" s="3">
         <v>92190651</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B148" s="4" t="s">
         <v>202</v>
       </c>
       <c r="C148" s="3">
@@ -3834,10 +3842,10 @@
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" s="3" t="s">
+      <c r="A149" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B149" s="4" t="s">
         <v>204</v>
       </c>
       <c r="C149" s="3">
@@ -3845,10 +3853,10 @@
       </c>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" s="3" t="s">
+      <c r="A150" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B150" s="3" t="s">
+      <c r="B150" s="4" t="s">
         <v>206</v>
       </c>
       <c r="C150" s="3">
@@ -3856,10 +3864,10 @@
       </c>
     </row>
     <row r="151" spans="1:3">
-      <c r="A151" s="3" t="s">
+      <c r="A151" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B151" s="4" t="s">
         <v>208</v>
       </c>
       <c r="C151" s="3">
@@ -3867,10 +3875,10 @@
       </c>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="3" t="s">
+      <c r="A152" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B152" s="3" t="s">
+      <c r="B152" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C152" s="3">
@@ -3878,10 +3886,10 @@
       </c>
     </row>
     <row r="153" spans="1:3">
-      <c r="A153" s="3" t="s">
+      <c r="A153" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B153" s="3" t="s">
+      <c r="B153" s="4" t="s">
         <v>212</v>
       </c>
       <c r="C153" s="3">
@@ -3889,10 +3897,10 @@
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="3" t="s">
+      <c r="A154" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B154" s="3" t="s">
+      <c r="B154" s="4" t="s">
         <v>214</v>
       </c>
       <c r="C154" s="3">
@@ -3900,10 +3908,10 @@
       </c>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155" s="3" t="s">
+      <c r="A155" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B155" s="4" t="s">
         <v>216</v>
       </c>
       <c r="C155" s="3">
@@ -3911,10 +3919,10 @@
       </c>
     </row>
     <row r="156" spans="1:3">
-      <c r="A156" s="3" t="s">
+      <c r="A156" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B156" s="4" t="s">
         <v>218</v>
       </c>
       <c r="C156" s="3">
@@ -3922,10 +3930,10 @@
       </c>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="3" t="s">
+      <c r="A157" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B157" s="3" t="s">
+      <c r="B157" s="4" t="s">
         <v>220</v>
       </c>
       <c r="C157" s="3">
@@ -3933,10 +3941,10 @@
       </c>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B158" s="3" t="s">
+      <c r="B158" s="4" t="s">
         <v>222</v>
       </c>
       <c r="C158" s="3">
@@ -3944,10 +3952,10 @@
       </c>
     </row>
     <row r="159" spans="1:3">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B159" s="3" t="s">
+      <c r="B159" s="4" t="s">
         <v>224</v>
       </c>
       <c r="C159" s="3">
@@ -3955,10 +3963,10 @@
       </c>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="B160" s="3" t="s">
+      <c r="B160" s="4" t="s">
         <v>226</v>
       </c>
       <c r="C160" s="3">
@@ -3969,7 +3977,7 @@
       <c r="A161" s="3">
         <v>92190652</v>
       </c>
-      <c r="B161" s="3" t="s">
+      <c r="B161" s="4" t="s">
         <v>227</v>
       </c>
       <c r="C161" s="3">
@@ -3980,7 +3988,7 @@
       <c r="A162" s="3">
         <v>92190653</v>
       </c>
-      <c r="B162" s="3" t="s">
+      <c r="B162" s="4" t="s">
         <v>228</v>
       </c>
       <c r="C162" s="3">
@@ -3991,7 +3999,7 @@
       <c r="A163" s="3">
         <v>92190654</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="B163" s="4" t="s">
         <v>229</v>
       </c>
       <c r="C163" s="3">
@@ -4002,7 +4010,7 @@
       <c r="A164" s="3">
         <v>92190655</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="B164" s="4" t="s">
         <v>230</v>
       </c>
       <c r="C164" s="3">
@@ -4013,7 +4021,7 @@
       <c r="A165" s="3">
         <v>92190656</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="B165" s="4" t="s">
         <v>231</v>
       </c>
       <c r="C165" s="3">
@@ -4024,7 +4032,7 @@
       <c r="A166" s="3">
         <v>92190659</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B166" s="4" t="s">
         <v>232</v>
       </c>
       <c r="C166" s="3">
@@ -4035,7 +4043,7 @@
       <c r="A167" s="3">
         <v>93000555</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B167" s="4" t="s">
         <v>233</v>
       </c>
       <c r="C167" s="3">
@@ -4046,7 +4054,7 @@
       <c r="A168" s="3">
         <v>93000556</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B168" s="4" t="s">
         <v>234</v>
       </c>
       <c r="C168" s="3">
@@ -4057,7 +4065,7 @@
       <c r="A169" s="3">
         <v>92065501</v>
       </c>
-      <c r="B169" s="3" t="s">
+      <c r="B169" s="4" t="s">
         <v>235</v>
       </c>
       <c r="C169" s="3">
@@ -4068,7 +4076,7 @@
       <c r="A170" s="3">
         <v>92065502</v>
       </c>
-      <c r="B170" s="3" t="s">
+      <c r="B170" s="4" t="s">
         <v>236</v>
       </c>
       <c r="C170" s="3">
@@ -4086,7 +4094,7 @@
       <c r="A172" s="3">
         <v>90681001</v>
       </c>
-      <c r="B172" s="3" t="s">
+      <c r="B172" s="4" t="s">
         <v>238</v>
       </c>
       <c r="C172" s="3">
@@ -4097,7 +4105,7 @@
       <c r="A173" s="3">
         <v>90681002</v>
       </c>
-      <c r="B173" s="3" t="s">
+      <c r="B173" s="4" t="s">
         <v>239</v>
       </c>
       <c r="C173" s="3">
@@ -4108,7 +4116,7 @@
       <c r="A174" s="3">
         <v>90681068</v>
       </c>
-      <c r="B174" s="3" t="s">
+      <c r="B174" s="4" t="s">
         <v>240</v>
       </c>
       <c r="C174" s="3">
@@ -4119,7 +4127,7 @@
       <c r="A175" s="3">
         <v>90681003</v>
       </c>
-      <c r="B175" s="3" t="s">
+      <c r="B175" s="4" t="s">
         <v>241</v>
       </c>
       <c r="C175" s="3">
@@ -4130,7 +4138,7 @@
       <c r="A176" s="3">
         <v>90681007</v>
       </c>
-      <c r="B176" s="3" t="s">
+      <c r="B176" s="4" t="s">
         <v>242</v>
       </c>
       <c r="C176" s="3">
@@ -4141,7 +4149,7 @@
       <c r="A177" s="3">
         <v>90681008</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="B177" s="4" t="s">
         <v>243</v>
       </c>
       <c r="C177" s="3">
@@ -4152,7 +4160,7 @@
       <c r="A178" s="3">
         <v>90681055</v>
       </c>
-      <c r="B178" s="3" t="s">
+      <c r="B178" s="4" t="s">
         <v>244</v>
       </c>
       <c r="C178" s="3">
@@ -4163,7 +4171,7 @@
       <c r="A179" s="3">
         <v>90681056</v>
       </c>
-      <c r="B179" s="3" t="s">
+      <c r="B179" s="4" t="s">
         <v>245</v>
       </c>
       <c r="C179" s="3">
@@ -4174,7 +4182,7 @@
       <c r="A180" s="3">
         <v>90681013</v>
       </c>
-      <c r="B180" s="3" t="s">
+      <c r="B180" s="4" t="s">
         <v>246</v>
       </c>
       <c r="C180" s="3">
@@ -4185,7 +4193,7 @@
       <c r="A181" s="3">
         <v>90681010</v>
       </c>
-      <c r="B181" s="3" t="s">
+      <c r="B181" s="4" t="s">
         <v>247</v>
       </c>
       <c r="C181" s="3">
@@ -4196,7 +4204,7 @@
       <c r="A182" s="3">
         <v>90681032</v>
       </c>
-      <c r="B182" s="3" t="s">
+      <c r="B182" s="4" t="s">
         <v>248</v>
       </c>
       <c r="C182" s="3">
@@ -4214,7 +4222,7 @@
       <c r="A184" s="3">
         <v>90555501</v>
       </c>
-      <c r="B184" s="3" t="s">
+      <c r="B184" s="4" t="s">
         <v>250</v>
       </c>
       <c r="C184" s="3">
@@ -4225,7 +4233,7 @@
       <c r="A185" s="3">
         <v>90555502</v>
       </c>
-      <c r="B185" s="3" t="s">
+      <c r="B185" s="4" t="s">
         <v>251</v>
       </c>
       <c r="C185" s="3">
@@ -4236,7 +4244,7 @@
       <c r="A186" s="3">
         <v>90555508</v>
       </c>
-      <c r="B186" s="3" t="s">
+      <c r="B186" s="4" t="s">
         <v>252</v>
       </c>
       <c r="C186" s="3">
@@ -4247,7 +4255,7 @@
       <c r="A187" s="3">
         <v>90555510</v>
       </c>
-      <c r="B187" s="3" t="s">
+      <c r="B187" s="4" t="s">
         <v>253</v>
       </c>
       <c r="C187" s="3">
@@ -4258,7 +4266,7 @@
       <c r="A188" s="3">
         <v>90555588</v>
       </c>
-      <c r="B188" s="3" t="s">
+      <c r="B188" s="4" t="s">
         <v>254</v>
       </c>
       <c r="C188" s="3">
@@ -4269,7 +4277,7 @@
       <c r="A189" s="3">
         <v>90555581</v>
       </c>
-      <c r="B189" s="3" t="s">
+      <c r="B189" s="4" t="s">
         <v>255</v>
       </c>
       <c r="C189" s="3">
@@ -4287,7 +4295,7 @@
       <c r="A191" s="3">
         <v>90112200</v>
       </c>
-      <c r="B191" s="3" t="s">
+      <c r="B191" s="4" t="s">
         <v>257</v>
       </c>
       <c r="C191" s="3">
@@ -4298,7 +4306,7 @@
       <c r="A192" s="3">
         <v>90112300</v>
       </c>
-      <c r="B192" s="3" t="s">
+      <c r="B192" s="4" t="s">
         <v>258</v>
       </c>
       <c r="C192" s="3">
@@ -4309,7 +4317,7 @@
       <c r="A193" s="3">
         <v>90112400</v>
       </c>
-      <c r="B193" s="3" t="s">
+      <c r="B193" s="4" t="s">
         <v>259</v>
       </c>
       <c r="C193" s="3">
@@ -4320,7 +4328,7 @@
       <c r="A194" s="3">
         <v>90114200</v>
       </c>
-      <c r="B194" s="3" t="s">
+      <c r="B194" s="4" t="s">
         <v>260</v>
       </c>
       <c r="C194" s="3">
@@ -4331,7 +4339,7 @@
       <c r="A195" s="3">
         <v>90114300</v>
       </c>
-      <c r="B195" s="3" t="s">
+      <c r="B195" s="4" t="s">
         <v>261</v>
       </c>
       <c r="C195" s="3">
@@ -4342,7 +4350,7 @@
       <c r="A196" s="3">
         <v>90114400</v>
       </c>
-      <c r="B196" s="3" t="s">
+      <c r="B196" s="4" t="s">
         <v>262</v>
       </c>
       <c r="C196" s="3">
@@ -4353,7 +4361,7 @@
       <c r="A197" s="3">
         <v>90114500</v>
       </c>
-      <c r="B197" s="3" t="s">
+      <c r="B197" s="4" t="s">
         <v>263</v>
       </c>
       <c r="C197" s="3">
@@ -4364,7 +4372,7 @@
       <c r="A198" s="3">
         <v>90114600</v>
       </c>
-      <c r="B198" s="3" t="s">
+      <c r="B198" s="4" t="s">
         <v>264</v>
       </c>
       <c r="C198" s="3">
@@ -4375,7 +4383,7 @@
       <c r="A199" s="3">
         <v>90116300</v>
       </c>
-      <c r="B199" s="3" t="s">
+      <c r="B199" s="4" t="s">
         <v>265</v>
       </c>
       <c r="C199" s="3">
@@ -4386,7 +4394,7 @@
       <c r="A200" s="3">
         <v>90118300</v>
       </c>
-      <c r="B200" s="3" t="s">
+      <c r="B200" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C200" s="3">
@@ -4397,7 +4405,7 @@
       <c r="A201" s="3">
         <v>90118500</v>
       </c>
-      <c r="B201" s="3" t="s">
+      <c r="B201" s="4" t="s">
         <v>267</v>
       </c>
       <c r="C201" s="3">
@@ -4408,7 +4416,7 @@
       <c r="A202" s="3">
         <v>90112202</v>
       </c>
-      <c r="B202" s="3" t="s">
+      <c r="B202" s="4" t="s">
         <v>268</v>
       </c>
       <c r="C202" s="3">
@@ -4419,7 +4427,7 @@
       <c r="A203" s="3">
         <v>90112203</v>
       </c>
-      <c r="B203" s="3" t="s">
+      <c r="B203" s="4" t="s">
         <v>269</v>
       </c>
       <c r="C203" s="3">
@@ -4430,7 +4438,7 @@
       <c r="A204" s="3">
         <v>90112205</v>
       </c>
-      <c r="B204" s="3" t="s">
+      <c r="B204" s="4" t="s">
         <v>270</v>
       </c>
       <c r="C204" s="3">
@@ -4441,7 +4449,7 @@
       <c r="A205" s="3">
         <v>90112302</v>
       </c>
-      <c r="B205" s="3" t="s">
+      <c r="B205" s="4" t="s">
         <v>271</v>
       </c>
       <c r="C205" s="3">
@@ -4452,7 +4460,7 @@
       <c r="A206" s="3">
         <v>90112303</v>
       </c>
-      <c r="B206" s="3" t="s">
+      <c r="B206" s="4" t="s">
         <v>272</v>
       </c>
       <c r="C206" s="3">
@@ -4463,7 +4471,7 @@
       <c r="A207" s="3">
         <v>90112305</v>
       </c>
-      <c r="B207" s="3" t="s">
+      <c r="B207" s="4" t="s">
         <v>273</v>
       </c>
       <c r="C207" s="3">
@@ -4474,7 +4482,7 @@
       <c r="A208" s="3">
         <v>90112403</v>
       </c>
-      <c r="B208" s="3" t="s">
+      <c r="B208" s="4" t="s">
         <v>274</v>
       </c>
       <c r="C208" s="3">
@@ -4485,7 +4493,7 @@
       <c r="A209" s="3">
         <v>90112405</v>
       </c>
-      <c r="B209" s="3" t="s">
+      <c r="B209" s="4" t="s">
         <v>275</v>
       </c>
       <c r="C209" s="3">
@@ -4503,7 +4511,7 @@
       <c r="A211" s="3">
         <v>90305400</v>
       </c>
-      <c r="B211" s="3" t="s">
+      <c r="B211" s="4" t="s">
         <v>277</v>
       </c>
       <c r="C211" s="3">
@@ -4514,7 +4522,7 @@
       <c r="A212" s="3">
         <v>90305410</v>
       </c>
-      <c r="B212" s="3" t="s">
+      <c r="B212" s="4" t="s">
         <v>278</v>
       </c>
       <c r="C212" s="3">
@@ -4525,7 +4533,7 @@
       <c r="A213" s="3">
         <v>90304100</v>
       </c>
-      <c r="B213" s="3" t="s">
+      <c r="B213" s="4" t="s">
         <v>279</v>
       </c>
       <c r="C213" s="3">
@@ -4536,7 +4544,7 @@
       <c r="A214" s="3">
         <v>90304200</v>
       </c>
-      <c r="B214" s="3" t="s">
+      <c r="B214" s="4" t="s">
         <v>280</v>
       </c>
       <c r="C214" s="3">
@@ -4547,7 +4555,7 @@
       <c r="A215" s="3">
         <v>90301805</v>
       </c>
-      <c r="B215" s="3" t="s">
+      <c r="B215" s="4" t="s">
         <v>281</v>
       </c>
       <c r="C215" s="3">
@@ -4558,7 +4566,7 @@
       <c r="A216" s="3">
         <v>90301815</v>
       </c>
-      <c r="B216" s="3" t="s">
+      <c r="B216" s="4" t="s">
         <v>282</v>
       </c>
       <c r="C216" s="3">
@@ -4569,7 +4577,7 @@
       <c r="A217" s="3">
         <v>90301800</v>
       </c>
-      <c r="B217" s="3" t="s">
+      <c r="B217" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C217" s="3">
@@ -4580,7 +4588,7 @@
       <c r="A218" s="3">
         <v>90302500</v>
       </c>
-      <c r="B218" s="3" t="s">
+      <c r="B218" s="4" t="s">
         <v>284</v>
       </c>
       <c r="C218" s="3">
@@ -4591,7 +4599,7 @@
       <c r="A219" s="3">
         <v>90303003</v>
       </c>
-      <c r="B219" s="3" t="s">
+      <c r="B219" s="4" t="s">
         <v>285</v>
       </c>
       <c r="C219" s="3">
@@ -4609,7 +4617,7 @@
       <c r="A221" s="3">
         <v>90912002</v>
       </c>
-      <c r="B221" s="3" t="s">
+      <c r="B221" s="4" t="s">
         <v>287</v>
       </c>
       <c r="C221" s="3">
@@ -4620,7 +4628,7 @@
       <c r="A222" s="3">
         <v>90912004</v>
       </c>
-      <c r="B222" s="3" t="s">
+      <c r="B222" s="4" t="s">
         <v>288</v>
       </c>
       <c r="C222" s="3">
@@ -4631,7 +4639,7 @@
       <c r="A223" s="3">
         <v>90912006</v>
       </c>
-      <c r="B223" s="3" t="s">
+      <c r="B223" s="4" t="s">
         <v>289</v>
       </c>
       <c r="C223" s="3">
@@ -4642,7 +4650,7 @@
       <c r="A224" s="3">
         <v>90912008</v>
       </c>
-      <c r="B224" s="3" t="s">
+      <c r="B224" s="4" t="s">
         <v>290</v>
       </c>
       <c r="C224" s="3">
@@ -4653,7 +4661,7 @@
       <c r="A225" s="3">
         <v>90912012</v>
       </c>
-      <c r="B225" s="3" t="s">
+      <c r="B225" s="4" t="s">
         <v>291</v>
       </c>
       <c r="C225" s="3">
@@ -4664,7 +4672,7 @@
       <c r="A226" s="3">
         <v>90912016</v>
       </c>
-      <c r="B226" s="3" t="s">
+      <c r="B226" s="4" t="s">
         <v>292</v>
       </c>
       <c r="C226" s="3">
@@ -4675,7 +4683,7 @@
       <c r="A227" s="3">
         <v>90912018</v>
       </c>
-      <c r="B227" s="3" t="s">
+      <c r="B227" s="4" t="s">
         <v>293</v>
       </c>
       <c r="C227" s="3">
@@ -4686,7 +4694,7 @@
       <c r="A228" s="3">
         <v>90912024</v>
       </c>
-      <c r="B228" s="3" t="s">
+      <c r="B228" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C228" s="3">
@@ -4697,7 +4705,7 @@
       <c r="A229" s="3">
         <v>90912036</v>
       </c>
-      <c r="B229" s="3" t="s">
+      <c r="B229" s="4" t="s">
         <v>295</v>
       </c>
       <c r="C229" s="3">
@@ -4708,7 +4716,7 @@
       <c r="A230" s="3">
         <v>90912102</v>
       </c>
-      <c r="B230" s="3" t="s">
+      <c r="B230" s="4" t="s">
         <v>296</v>
       </c>
       <c r="C230" s="3">
@@ -4719,7 +4727,7 @@
       <c r="A231" s="3">
         <v>90912104</v>
       </c>
-      <c r="B231" s="3" t="s">
+      <c r="B231" s="4" t="s">
         <v>297</v>
       </c>
       <c r="C231" s="3">
@@ -4730,7 +4738,7 @@
       <c r="A232" s="3">
         <v>90912106</v>
       </c>
-      <c r="B232" s="3" t="s">
+      <c r="B232" s="4" t="s">
         <v>298</v>
       </c>
       <c r="C232" s="3">
@@ -4741,7 +4749,7 @@
       <c r="A233" s="3">
         <v>90912108</v>
       </c>
-      <c r="B233" s="3" t="s">
+      <c r="B233" s="4" t="s">
         <v>299</v>
       </c>
       <c r="C233" s="3">
@@ -4752,7 +4760,7 @@
       <c r="A234" s="3">
         <v>90912112</v>
       </c>
-      <c r="B234" s="3" t="s">
+      <c r="B234" s="4" t="s">
         <v>300</v>
       </c>
       <c r="C234" s="3">
@@ -4763,7 +4771,7 @@
       <c r="A235" s="3">
         <v>90912116</v>
       </c>
-      <c r="B235" s="3" t="s">
+      <c r="B235" s="4" t="s">
         <v>301</v>
       </c>
       <c r="C235" s="3">
@@ -4774,7 +4782,7 @@
       <c r="A236" s="3">
         <v>90912118</v>
       </c>
-      <c r="B236" s="3" t="s">
+      <c r="B236" s="4" t="s">
         <v>302</v>
       </c>
       <c r="C236" s="3">
@@ -4785,7 +4793,7 @@
       <c r="A237" s="3">
         <v>90912124</v>
       </c>
-      <c r="B237" s="3" t="s">
+      <c r="B237" s="4" t="s">
         <v>303</v>
       </c>
       <c r="C237" s="3">
@@ -4796,7 +4804,7 @@
       <c r="A238" s="3">
         <v>90912136</v>
       </c>
-      <c r="B238" s="3" t="s">
+      <c r="B238" s="4" t="s">
         <v>304</v>
       </c>
       <c r="C238" s="3">
@@ -4807,7 +4815,7 @@
       <c r="A239" s="3">
         <v>90914000</v>
       </c>
-      <c r="B239" s="3" t="s">
+      <c r="B239" s="4" t="s">
         <v>305</v>
       </c>
       <c r="C239" s="3">
@@ -4818,7 +4826,7 @@
       <c r="A240" s="3">
         <v>90914001</v>
       </c>
-      <c r="B240" s="3" t="s">
+      <c r="B240" s="4" t="s">
         <v>306</v>
       </c>
       <c r="C240" s="3">
@@ -4829,7 +4837,7 @@
       <c r="A241" s="3">
         <v>90914003</v>
       </c>
-      <c r="B241" s="3" t="s">
+      <c r="B241" s="4" t="s">
         <v>307</v>
       </c>
       <c r="C241" s="3">
@@ -4844,10 +4852,10 @@
       <c r="C242" s="1"/>
     </row>
     <row r="243" spans="1:3">
-      <c r="A243" s="3" t="s">
+      <c r="A243" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B243" s="3" t="s">
+      <c r="B243" s="4" t="s">
         <v>310</v>
       </c>
       <c r="C243" s="3">
@@ -4855,10 +4863,10 @@
       </c>
     </row>
     <row r="244" spans="1:3">
-      <c r="A244" s="3" t="s">
+      <c r="A244" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="B244" s="3" t="s">
+      <c r="B244" s="4" t="s">
         <v>312</v>
       </c>
       <c r="C244" s="3">
@@ -4866,10 +4874,10 @@
       </c>
     </row>
     <row r="245" spans="1:3">
-      <c r="A245" s="3" t="s">
+      <c r="A245" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B245" s="3" t="s">
+      <c r="B245" s="4" t="s">
         <v>314</v>
       </c>
       <c r="C245" s="3">
@@ -4877,10 +4885,10 @@
       </c>
     </row>
     <row r="246" spans="1:3">
-      <c r="A246" s="3" t="s">
+      <c r="A246" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B246" s="3" t="s">
+      <c r="B246" s="4" t="s">
         <v>316</v>
       </c>
       <c r="C246" s="3">
@@ -4888,10 +4896,10 @@
       </c>
     </row>
     <row r="247" spans="1:3">
-      <c r="A247" s="3" t="s">
+      <c r="A247" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="B247" s="3" t="s">
+      <c r="B247" s="4" t="s">
         <v>318</v>
       </c>
       <c r="C247" s="3">
@@ -4899,10 +4907,10 @@
       </c>
     </row>
     <row r="248" spans="1:3">
-      <c r="A248" s="3" t="s">
+      <c r="A248" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B248" s="3" t="s">
+      <c r="B248" s="4" t="s">
         <v>320</v>
       </c>
       <c r="C248" s="3">
@@ -4910,10 +4918,10 @@
       </c>
     </row>
     <row r="249" spans="1:3">
-      <c r="A249" s="3" t="s">
+      <c r="A249" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="B249" s="3" t="s">
+      <c r="B249" s="4" t="s">
         <v>322</v>
       </c>
       <c r="C249" s="3">
@@ -4921,10 +4929,10 @@
       </c>
     </row>
     <row r="250" spans="1:3">
-      <c r="A250" s="3" t="s">
+      <c r="A250" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="B250" s="3" t="s">
+      <c r="B250" s="4" t="s">
         <v>324</v>
       </c>
       <c r="C250" s="3">
@@ -4932,10 +4940,10 @@
       </c>
     </row>
     <row r="251" spans="1:3">
-      <c r="A251" s="3" t="s">
+      <c r="A251" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="B251" s="3" t="s">
+      <c r="B251" s="4" t="s">
         <v>326</v>
       </c>
       <c r="C251" s="3">
@@ -4943,10 +4951,10 @@
       </c>
     </row>
     <row r="252" spans="1:3">
-      <c r="A252" s="3" t="s">
+      <c r="A252" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="B252" s="3" t="s">
+      <c r="B252" s="4" t="s">
         <v>328</v>
       </c>
       <c r="C252" s="3">
@@ -4954,10 +4962,10 @@
       </c>
     </row>
     <row r="253" spans="1:3">
-      <c r="A253" s="3" t="s">
+      <c r="A253" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B253" s="3" t="s">
+      <c r="B253" s="4" t="s">
         <v>330</v>
       </c>
       <c r="C253" s="3">
@@ -4965,10 +4973,10 @@
       </c>
     </row>
     <row r="254" spans="1:3">
-      <c r="A254" s="3" t="s">
+      <c r="A254" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="B254" s="3" t="s">
+      <c r="B254" s="4" t="s">
         <v>332</v>
       </c>
       <c r="C254" s="3">
@@ -4976,10 +4984,10 @@
       </c>
     </row>
     <row r="255" spans="1:3">
-      <c r="A255" s="3" t="s">
+      <c r="A255" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B255" s="3" t="s">
+      <c r="B255" s="4" t="s">
         <v>334</v>
       </c>
       <c r="C255" s="3">
@@ -4987,10 +4995,10 @@
       </c>
     </row>
     <row r="256" spans="1:3">
-      <c r="A256" s="3" t="s">
+      <c r="A256" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="B256" s="3" t="s">
+      <c r="B256" s="4" t="s">
         <v>336</v>
       </c>
       <c r="C256" s="3">
@@ -4998,10 +5006,10 @@
       </c>
     </row>
     <row r="257" spans="1:3">
-      <c r="A257" s="3" t="s">
+      <c r="A257" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="B257" s="3" t="s">
+      <c r="B257" s="4" t="s">
         <v>338</v>
       </c>
       <c r="C257" s="3">
@@ -5009,10 +5017,10 @@
       </c>
     </row>
     <row r="258" spans="1:3">
-      <c r="A258" s="3" t="s">
+      <c r="A258" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B258" s="3" t="s">
+      <c r="B258" s="4" t="s">
         <v>340</v>
       </c>
       <c r="C258" s="3">
@@ -5020,10 +5028,10 @@
       </c>
     </row>
     <row r="259" spans="1:3">
-      <c r="A259" s="3" t="s">
+      <c r="A259" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="B259" s="3" t="s">
+      <c r="B259" s="4" t="s">
         <v>342</v>
       </c>
       <c r="C259" s="3">
@@ -5031,10 +5039,10 @@
       </c>
     </row>
     <row r="260" spans="1:3">
-      <c r="A260" s="3" t="s">
+      <c r="A260" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="B260" s="3" t="s">
+      <c r="B260" s="4" t="s">
         <v>344</v>
       </c>
       <c r="C260" s="3">
@@ -5042,10 +5050,10 @@
       </c>
     </row>
     <row r="261" spans="1:3">
-      <c r="A261" s="3" t="s">
+      <c r="A261" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="B261" s="3" t="s">
+      <c r="B261" s="4" t="s">
         <v>346</v>
       </c>
       <c r="C261" s="3">
@@ -5053,10 +5061,10 @@
       </c>
     </row>
     <row r="262" spans="1:3">
-      <c r="A262" s="3" t="s">
+      <c r="A262" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="B262" s="3" t="s">
+      <c r="B262" s="4" t="s">
         <v>348</v>
       </c>
       <c r="C262" s="3">
@@ -5064,10 +5072,10 @@
       </c>
     </row>
     <row r="263" spans="1:3">
-      <c r="A263" s="3" t="s">
+      <c r="A263" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="B263" s="3" t="s">
+      <c r="B263" s="4" t="s">
         <v>350</v>
       </c>
       <c r="C263" s="3">
@@ -5075,10 +5083,10 @@
       </c>
     </row>
     <row r="264" spans="1:3">
-      <c r="A264" s="3" t="s">
+      <c r="A264" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B264" s="3" t="s">
+      <c r="B264" s="4" t="s">
         <v>352</v>
       </c>
       <c r="C264" s="3">
@@ -5086,10 +5094,10 @@
       </c>
     </row>
     <row r="265" spans="1:3">
-      <c r="A265" s="3" t="s">
+      <c r="A265" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="B265" s="3" t="s">
+      <c r="B265" s="4" t="s">
         <v>354</v>
       </c>
       <c r="C265" s="3">
@@ -5097,10 +5105,10 @@
       </c>
     </row>
     <row r="266" spans="1:3">
-      <c r="A266" s="3" t="s">
+      <c r="A266" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="B266" s="3" t="s">
+      <c r="B266" s="4" t="s">
         <v>356</v>
       </c>
       <c r="C266" s="3">
@@ -5108,10 +5116,10 @@
       </c>
     </row>
     <row r="267" spans="1:3">
-      <c r="A267" s="3" t="s">
+      <c r="A267" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="B267" s="3" t="s">
+      <c r="B267" s="4" t="s">
         <v>358</v>
       </c>
       <c r="C267" s="3">
@@ -5119,10 +5127,10 @@
       </c>
     </row>
     <row r="268" spans="1:3">
-      <c r="A268" s="3" t="s">
+      <c r="A268" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B268" s="3" t="s">
+      <c r="B268" s="4" t="s">
         <v>360</v>
       </c>
       <c r="C268" s="3">
@@ -5130,10 +5138,10 @@
       </c>
     </row>
     <row r="269" spans="1:3">
-      <c r="A269" s="3" t="s">
+      <c r="A269" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="B269" s="3" t="s">
+      <c r="B269" s="4" t="s">
         <v>362</v>
       </c>
       <c r="C269" s="3">
@@ -5141,10 +5149,10 @@
       </c>
     </row>
     <row r="270" spans="1:3">
-      <c r="A270" s="3" t="s">
+      <c r="A270" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B270" s="3" t="s">
+      <c r="B270" s="4" t="s">
         <v>364</v>
       </c>
       <c r="C270" s="3">
@@ -5152,10 +5160,10 @@
       </c>
     </row>
     <row r="271" spans="1:3">
-      <c r="A271" s="3" t="s">
+      <c r="A271" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="B271" s="3" t="s">
+      <c r="B271" s="4" t="s">
         <v>366</v>
       </c>
       <c r="C271" s="3">
@@ -5163,10 +5171,10 @@
       </c>
     </row>
     <row r="272" spans="1:3">
-      <c r="A272" s="3" t="s">
+      <c r="A272" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="B272" s="3" t="s">
+      <c r="B272" s="4" t="s">
         <v>368</v>
       </c>
       <c r="C272" s="3">
@@ -5174,10 +5182,10 @@
       </c>
     </row>
     <row r="273" spans="1:3">
-      <c r="A273" s="3" t="s">
+      <c r="A273" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="B273" s="3" t="s">
+      <c r="B273" s="4" t="s">
         <v>370</v>
       </c>
       <c r="C273" s="3">
@@ -5185,10 +5193,10 @@
       </c>
     </row>
     <row r="274" spans="1:3">
-      <c r="A274" s="3" t="s">
+      <c r="A274" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="B274" s="3" t="s">
+      <c r="B274" s="4" t="s">
         <v>372</v>
       </c>
       <c r="C274" s="3">
@@ -5196,10 +5204,10 @@
       </c>
     </row>
     <row r="275" spans="1:3">
-      <c r="A275" s="3" t="s">
+      <c r="A275" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="B275" s="3" t="s">
+      <c r="B275" s="4" t="s">
         <v>374</v>
       </c>
       <c r="C275" s="3">
@@ -5207,10 +5215,10 @@
       </c>
     </row>
     <row r="276" spans="1:3">
-      <c r="A276" s="3" t="s">
+      <c r="A276" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="B276" s="3" t="s">
+      <c r="B276" s="4" t="s">
         <v>376</v>
       </c>
       <c r="C276" s="3">
@@ -5218,10 +5226,10 @@
       </c>
     </row>
     <row r="277" spans="1:3">
-      <c r="A277" s="3" t="s">
+      <c r="A277" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="B277" s="3" t="s">
+      <c r="B277" s="4" t="s">
         <v>378</v>
       </c>
       <c r="C277" s="3">
@@ -5229,10 +5237,10 @@
       </c>
     </row>
     <row r="278" spans="1:3">
-      <c r="A278" s="3" t="s">
+      <c r="A278" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="B278" s="3" t="s">
+      <c r="B278" s="4" t="s">
         <v>380</v>
       </c>
       <c r="C278" s="3">
@@ -5240,10 +5248,10 @@
       </c>
     </row>
     <row r="279" spans="1:3">
-      <c r="A279" s="3" t="s">
+      <c r="A279" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B279" s="3" t="s">
+      <c r="B279" s="4" t="s">
         <v>382</v>
       </c>
       <c r="C279" s="3">
@@ -5251,10 +5259,10 @@
       </c>
     </row>
     <row r="280" spans="1:3">
-      <c r="A280" s="3" t="s">
+      <c r="A280" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="B280" s="3" t="s">
+      <c r="B280" s="4" t="s">
         <v>384</v>
       </c>
       <c r="C280" s="3">
@@ -5262,10 +5270,10 @@
       </c>
     </row>
     <row r="281" spans="1:3">
-      <c r="A281" s="3" t="s">
+      <c r="A281" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="B281" s="3" t="s">
+      <c r="B281" s="4" t="s">
         <v>386</v>
       </c>
       <c r="C281" s="3">
@@ -5273,10 +5281,10 @@
       </c>
     </row>
     <row r="282" spans="1:3">
-      <c r="A282" s="3" t="s">
+      <c r="A282" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B282" s="3" t="s">
+      <c r="B282" s="4" t="s">
         <v>388</v>
       </c>
       <c r="C282" s="3">
@@ -5284,10 +5292,10 @@
       </c>
     </row>
     <row r="283" spans="1:3">
-      <c r="A283" s="3" t="s">
+      <c r="A283" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="B283" s="3" t="s">
+      <c r="B283" s="4" t="s">
         <v>390</v>
       </c>
       <c r="C283" s="3">
@@ -5295,10 +5303,10 @@
       </c>
     </row>
     <row r="284" spans="1:3">
-      <c r="A284" s="3" t="s">
+      <c r="A284" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="B284" s="3" t="s">
+      <c r="B284" s="4" t="s">
         <v>392</v>
       </c>
       <c r="C284" s="3">
@@ -5306,10 +5314,10 @@
       </c>
     </row>
     <row r="285" spans="1:3">
-      <c r="A285" s="3" t="s">
+      <c r="A285" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="B285" s="3" t="s">
+      <c r="B285" s="4" t="s">
         <v>394</v>
       </c>
       <c r="C285" s="3">
@@ -5317,10 +5325,10 @@
       </c>
     </row>
     <row r="286" spans="1:3">
-      <c r="A286" s="3" t="s">
+      <c r="A286" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="B286" s="3" t="s">
+      <c r="B286" s="4" t="s">
         <v>396</v>
       </c>
       <c r="C286" s="3">
@@ -5328,10 +5336,10 @@
       </c>
     </row>
     <row r="287" spans="1:3">
-      <c r="A287" s="3" t="s">
+      <c r="A287" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="B287" s="3" t="s">
+      <c r="B287" s="4" t="s">
         <v>398</v>
       </c>
       <c r="C287" s="3">

</xml_diff>